<commit_message>
Suite fabrication 2025 (ajout d'info)
</commit_message>
<xml_diff>
--- a/oyas/slaves_rs485/fabrication/modele_2024/nomenclature.xlsx
+++ b/oyas/slaves_rs485/fabrication/modele_2024/nomenclature.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\GITHUB\modules_uino\jarduino2\jard_485_slave\fabrication\modele_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\GITHUB\jarduino\oyas\slaves_rs485\fabrication\modele_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1BAC7B-E60C-48C8-88F2-0ED0C662F063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3DAD73-56FB-40A2-B129-18B36DBC3DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38550" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nomenclature 2024" sheetId="1" r:id="rId1"/>
+    <sheet name="Détails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>PU</t>
   </si>
@@ -53,9 +54,6 @@
     <t>Oya</t>
   </si>
   <si>
-    <t>Capteur de niveau</t>
-  </si>
-  <si>
     <t>Boîte de dérivation ronde</t>
   </si>
   <si>
@@ -74,35 +72,75 @@
     <t>Coude 10mm / 12mm</t>
   </si>
   <si>
-    <t>Collier 10mm</t>
-  </si>
-  <si>
     <t>Composants électroniques</t>
   </si>
   <si>
     <t>PCB</t>
   </si>
   <si>
-    <t>Cosses</t>
-  </si>
-  <si>
     <t>Embout tuyau 10mm sur 6cm</t>
   </si>
   <si>
     <t>Couvercle / soucoupe 17mm</t>
   </si>
   <si>
-    <t>Electrovanne 12V</t>
-  </si>
-  <si>
-    <t>Couple connecteurs étanche bus</t>
+    <t>Lien achat</t>
+  </si>
+  <si>
+    <t>Botanic</t>
+  </si>
+  <si>
+    <r>
+      <t>Capteur de niveau - Modèle</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200mm</t>
+    </r>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/4000467977004.html</t>
+  </si>
+  <si>
+    <t>Electrovanne 12V diam. 12mm</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/4000185704146.html</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/1005007995094485.html</t>
+  </si>
+  <si>
+    <t>Cosse 6.3mm</t>
+  </si>
+  <si>
+    <t>Collier 10mm - 16mm</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/1005004790494883.html</t>
+  </si>
+  <si>
+    <t>Castorama</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/4000029686070.html</t>
+  </si>
+  <si>
+    <t>Couple de connecteurs étanche bus (4 voies)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +170,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -150,17 +196,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -174,6 +222,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>40102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E4D4ED9-2653-3DBF-929C-F4566D03BA45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171451" y="85725"/>
+          <a:ext cx="6210300" cy="2621377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7196E9F5-00D0-1000-9871-A8BDC3D96E89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6524624" y="161924"/>
+          <a:ext cx="7362825" cy="2663293"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>485773</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FFA554A-AC29-C8DB-7DF6-CCE157055C93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14201773" y="247648"/>
+          <a:ext cx="914401" cy="914401"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>156709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38645</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D39B20A-F375-8574-8F24-29598ACA213E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238126" y="3014209"/>
+          <a:ext cx="6172200" cy="2358436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>706246</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95658</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6656355B-F145-E7B9-E74A-7503932BA559}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629399" y="3375928"/>
+          <a:ext cx="7030847" cy="2053730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,18 +712,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -463,10 +737,13 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>44.61</v>
@@ -479,9 +756,9 @@
         <v>44.61</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>5.52</v>
@@ -494,7 +771,7 @@
         <v>5.52</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -505,10 +782,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2.9</v>
@@ -520,40 +800,49 @@
         <f t="shared" si="0"/>
         <v>2.9</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>6.24</v>
+        <v>7.19</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>6.24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>7.19</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>4.6399999999999997</v>
+        <v>6.13</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>4.6399999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>6.13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -565,10 +854,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -580,26 +872,31 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <f>1.76/50</f>
-        <v>3.5200000000000002E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>7.0400000000000004E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <v>0.2</v>
@@ -612,9 +909,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <v>0.04</v>
@@ -627,9 +924,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <v>0.2</v>
@@ -642,9 +939,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>0.14000000000000001</v>
@@ -657,24 +954,27 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3">
-        <v>0.29199999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.58399999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3">
         <v>0.29199999999999998</v>
@@ -687,49 +987,65 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>19</v>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>27</v>
       </c>
       <c r="C18" s="3">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
+        <v>1.83</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.83</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="1">
         <f>SUM(E3:E18)</f>
-        <v>72.736400000000003</v>
+        <v>74.683999999999997</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{18ECABFE-3271-46A1-B6D3-9884EC74CAB6}"/>
+    <hyperlink ref="G8" r:id="rId2" xr:uid="{47D93D94-BFFB-424D-9470-45C051E34B1E}"/>
+    <hyperlink ref="G11" r:id="rId3" xr:uid="{D50232EC-9BAD-4B67-B212-BD3B3F8A96DC}"/>
+    <hyperlink ref="G16" r:id="rId4" xr:uid="{6CC23387-5381-41D7-A95E-AE4020F697EC}"/>
+    <hyperlink ref="G18" r:id="rId5" xr:uid="{ACED4528-34AC-4EE9-B7BB-4444F02BC788}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E4BE9A-71B1-49E4-B771-9DCD69805F7A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>